<commit_message>
FINAL V1.1 - Fixed test sequence numbering and updated testplan
</commit_message>
<xml_diff>
--- a/SV/testplan.xlsx
+++ b/SV/testplan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="117">
   <si>
     <t xml:space="preserve">Test Category</t>
   </si>
@@ -235,6 +235,9 @@
     <t xml:space="preserve">@negedge sclk, done_tx/done_rx should be asserted at the next posedge of clk </t>
   </si>
   <si>
+    <t xml:space="preserve">Duplex not done</t>
+  </si>
+  <si>
     <t xml:space="preserve">Internal Signals</t>
   </si>
   <si>
@@ -248,9 +251,6 @@
   </si>
   <si>
     <t xml:space="preserve">@negedge sclk_en, cs should be asserted at the next posedge of clk </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aiman</t>
   </si>
   <si>
     <t xml:space="preserve">sclk should update sclk_en</t>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t xml:space="preserve">Randomise the input and output should be following the input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aiman</t>
   </si>
   <si>
     <t xml:space="preserve">Error Handling (Mid-Transfer Reset)</t>
@@ -522,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -639,6 +642,20 @@
       <left/>
       <right style="hair"/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -689,7 +706,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -818,11 +835,31 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -908,7 +945,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -920,7 +957,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="61.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="59.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="3" width="9.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="11" style="3" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="4" width="11.52"/>
   </cols>
   <sheetData>
@@ -1142,11 +1181,14 @@
       <c r="I8" s="23" t="n">
         <v>0.5</v>
       </c>
+      <c r="J8" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="AMJ8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>5.1</v>
@@ -1155,19 +1197,25 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>46</v>
+        <v>16</v>
+      </c>
+      <c r="I9" s="25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,44 +1425,46 @@
         <v>78</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="29"/>
+        <v>79</v>
+      </c>
+      <c r="I17" s="29" t="n">
+        <v>1</v>
+      </c>
       <c r="AMJ17" s="4"/>
     </row>
-    <row r="18" s="12" customFormat="true" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="11" t="n">
+    <row r="18" s="16" customFormat="true" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="31" t="n">
         <v>7.1</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="E18" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="F18" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="G18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="19" t="n">
+      <c r="I18" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="AMJ18" s="4"/>
+      <c r="AMJ18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="46.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>7.2</v>
@@ -1423,50 +1473,50 @@
         <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" s="32" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="s">
+      <c r="I19" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="31" t="n">
+    </row>
+    <row r="20" s="37" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="36" t="n">
         <v>8.1</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="32" t="s">
+      <c r="C20" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="D20" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="E20" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="F20" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="33" t="n">
+      <c r="G20" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="38" t="n">
         <v>1</v>
       </c>
       <c r="AMJ20" s="8"/>
@@ -1502,7 +1552,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.01"/>
@@ -1512,22 +1562,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,19 +1585,19 @@
         <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,19 +1605,19 @@
         <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,19 +1625,19 @@
         <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>